<commit_message>
echomri data fixed 3
</commit_message>
<xml_diff>
--- a/data/echoMRI/Kotz07162025.xlsx
+++ b/data/echoMRI/Kotz07162025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcaballero/Documents/GitHub/data/data/echoMRI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512C7AFE-6AAF-A94F-891E-76C7380000E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869D5935-C320-684F-B9C9-67926C4B5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
     <t>14:06:09 Jul 16, 2025; 27; ems</t>
   </si>
   <si>
-    <t>14:07:25 16 Jul 16, 2025; 31; ems</t>
+    <t>14:07:25 Jul 16, 2025; 31; ems</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>